<commit_message>
added more line id stuff
</commit_message>
<xml_diff>
--- a/Abundance_Estimation_EW/norm_RVcorr_LHS72.txt_EWs.xlsx
+++ b/Abundance_Estimation_EW/norm_RVcorr_LHS72.txt_EWs.xlsx
@@ -1,37 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapta\Desktop\Atmospheric_Studies_VLMS\Abundance_Estimation_EW\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E906178-3C1E-4A0E-B355-F45197159CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
-  <si>
-    <t>wave</t>
-  </si>
-  <si>
-    <t>blue_end</t>
-  </si>
-  <si>
-    <t>red_end</t>
-  </si>
-  <si>
-    <t>profile</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+  <si>
+    <t>Absorption_Lines_(A)</t>
+  </si>
+  <si>
+    <t>Closest_NIST_Wavelength_(A)</t>
+  </si>
+  <si>
+    <t>Corresponding_Ion</t>
+  </si>
+  <si>
+    <t>Blue_end</t>
+  </si>
+  <si>
+    <t>Red_end</t>
+  </si>
+  <si>
+    <t>Profile</t>
   </si>
   <si>
     <t>EW</t>
   </si>
   <si>
     <t>EW Error</t>
+  </si>
+  <si>
+    <t>Ca I</t>
   </si>
   <si>
     <t>Lorentzian</t>
@@ -46,17 +61,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,27 +79,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -101,7 +93,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -110,6 +102,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -156,7 +156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +188,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +240,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,14 +433,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,188 +471,249 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>6464.353</v>
+        <v>6464.3275249999997</v>
       </c>
       <c r="B2">
+        <v>6464.3530000000001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>6463.3</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>6465.17</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>0.3392683210255918</v>
-      </c>
-      <c r="F2">
-        <v>0.01162605570619592</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>0.33926832102559179</v>
+      </c>
+      <c r="H2">
+        <v>1.1626055706195919E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>6473.4173870000004</v>
+      </c>
+      <c r="B3">
         <v>6473.45</v>
       </c>
-      <c r="B3">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
         <v>6472.7</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>6474.4</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>0.1868150184789328</v>
-      </c>
-      <c r="F3">
-        <v>0.005551126884089422</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>0.18681501847893281</v>
+      </c>
+      <c r="H3">
+        <v>5.5511268840894223E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>6495.5543340000004</v>
+      </c>
+      <c r="B4">
         <v>6495.576</v>
       </c>
-      <c r="B4">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>6494.5</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>6497.7</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>0.2893414043683777</v>
-      </c>
-      <c r="F4">
-        <v>0.0144497247223063</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>0.28934140436837769</v>
+      </c>
+      <c r="H4">
+        <v>1.44497247223063E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>6501.446</v>
+        <v>6501.4118090000002</v>
       </c>
       <c r="B5">
+        <v>6501.4459999999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
         <v>6500.2</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>6502.8</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>0.1438560354000702</v>
-      </c>
-      <c r="F5">
-        <v>0.006473211215864163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.14385603540007019</v>
+      </c>
+      <c r="H5">
+        <v>6.4732112158641629E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6574.595</v>
+        <v>6574.561686</v>
       </c>
       <c r="B6">
+        <v>6574.5950000000003</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
         <v>6573.7</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>6575.4</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
         <v>0.1393475869694169</v>
       </c>
-      <c r="F6">
-        <v>0.003752187920412557</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6">
+        <v>3.7521879204125571E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6719.536</v>
+        <v>6719.5097159999996</v>
       </c>
       <c r="B7">
+        <v>6719.5360000000001</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
         <v>6718.3</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>6720.8</v>
       </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
         <v>0.2157192683602569</v>
       </c>
-      <c r="F7">
-        <v>0.008534130340982975</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7">
+        <v>8.5341303409829754E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>7150.1027260000001</v>
+      </c>
+      <c r="B8">
         <v>7150</v>
       </c>
-      <c r="B8">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
         <v>7149</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>7151.7</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>0.2979109547955234</v>
-      </c>
-      <c r="F8">
-        <v>0.01273121621722973</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>0.29791095479552337</v>
+      </c>
+      <c r="H8">
+        <v>1.2731216217229731E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>7204.1521389999998</v>
+      </c>
+      <c r="B9">
         <v>7204</v>
       </c>
-      <c r="B9">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
         <v>7203</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>7206.4</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>0.2247352142435375</v>
-      </c>
-      <c r="F9">
-        <v>0.01196891326161377</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>0.22473521424353751</v>
+      </c>
+      <c r="H9">
+        <v>1.196891326161377E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>7328.1386339999999</v>
+      </c>
+      <c r="B10">
         <v>7328</v>
       </c>
-      <c r="B10">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
         <v>7327</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>7329.5</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <v>0.2512544933567619</v>
-      </c>
-      <c r="F10">
-        <v>0.01016079138694332</v>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>0.25125449335676192</v>
+      </c>
+      <c r="H10">
+        <v>1.016079138694332E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>